<commit_message>
Incorporate EU cost pass-through shares for glass, cement, and steel. Assume others remain at 100% unless other EU-specific sources are found
</commit_message>
<xml_diff>
--- a/InputData/indst/SoCiIEPTtB/Shr of Cng in Indst Expenses Passed Thr to Buyers.xlsx
+++ b/InputData/indst/SoCiIEPTtB/Shr of Cng in Indst Expenses Passed Thr to Buyers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\U.S. Models\eps-us\InputData\indst\SoCiIEPTtB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\indst\SoCiIEPTtB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D87643-3FBD-4818-AB4B-E532AC1F3B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE4A1B8-3AA4-4856-A846-0C4E2DB475ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35730" yWindow="4035" windowWidth="21600" windowHeight="12525" activeTab="1" xr2:uid="{C45C27AA-02D4-49AC-94B3-A048BBC9260E}"/>
+    <workbookView xWindow="30690" yWindow="4170" windowWidth="21585" windowHeight="12525" activeTab="1" xr2:uid="{C45C27AA-02D4-49AC-94B3-A048BBC9260E}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>SoCiIEPTtB Share of Change in Industry Expenses Passed Through to Buyers</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Accordingly, we adopt the recommendation of the Benedek, de Mooij, Keen, &amp; Wingender (2015) study</t>
   </si>
   <si>
-    <t>and assume full passthrough.</t>
-  </si>
-  <si>
     <t>Share of cost increases passed through to consumers</t>
   </si>
   <si>
@@ -214,6 +211,24 @@
   </si>
   <si>
     <t>construction 41T43</t>
+  </si>
+  <si>
+    <t>and assume full passthrough for many industries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the EU, however, we have found ETS to greatly impact prices, and therefore demand, imports, and exports. </t>
+  </si>
+  <si>
+    <t>Cludius et al.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.eneco.2020.104883</t>
+  </si>
+  <si>
+    <t>Ex-post investigation of cost pass-through in the EU ETS - an analysis for six industry sectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a result, we use estimated values from Cludius et al. for some industries. </t>
   </si>
 </sst>
 </file>
@@ -597,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA9904B-1EB4-4402-820D-BB1B47048552}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,141 +657,171 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
-        <v>32</v>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -796,7 +841,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -807,234 +852,231 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13">
-        <f>About!A$42</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14">
-        <f>About!A$42</f>
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15">
-        <f>About!A$42</f>
-        <v>1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26">
-        <f>About!A$42</f>
+        <f>About!A$47</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>